<commit_message>
added better read me file
</commit_message>
<xml_diff>
--- a/data/Freq_Phase_Data.xlsx
+++ b/data/Freq_Phase_Data.xlsx
@@ -28,7 +28,1447 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="1080">
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
   <si>
     <t>Frequency</t>
   </si>
@@ -1888,28 +3328,28 @@
   <sheetData>
     <row r="1">
       <c r="C1" s="0" t="s">
-        <v>544</v>
+        <v>1024</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>545</v>
+        <v>1025</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>546</v>
+        <v>1026</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>547</v>
+        <v>1027</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>548</v>
+        <v>1028</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>549</v>
+        <v>1029</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>550</v>
+        <v>1030</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>551</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="2">
@@ -1923,7 +3363,7 @@
         <v>2.5</v>
       </c>
       <c r="G2" s="0">
-        <v>-1.4966853344018418</v>
+        <v>-1.4966850383464922</v>
       </c>
       <c r="I2" s="0">
         <v>2.75</v>
@@ -1949,7 +3389,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="0">
-        <v>-0.76308143485732693</v>
+        <v>-0.76308077159058862</v>
       </c>
       <c r="I3" s="0">
         <v>19.25</v>
@@ -1975,7 +3415,7 @@
         <v>0.25</v>
       </c>
       <c r="G4" s="0">
-        <v>0.41620960835448156</v>
+        <v>0.41620946961464156</v>
       </c>
       <c r="I4" s="0">
         <v>4.75</v>
@@ -2001,7 +3441,7 @@
         <v>0.75</v>
       </c>
       <c r="G5" s="0">
-        <v>-0.19802556824467418</v>
+        <v>-0.19802599720565486</v>
       </c>
       <c r="I5" s="0">
         <v>4</v>
@@ -2037,28 +3477,28 @@
   <sheetData>
     <row r="1">
       <c r="C1" s="0" t="s">
-        <v>552</v>
+        <v>1032</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>553</v>
+        <v>1033</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>554</v>
+        <v>1034</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>555</v>
+        <v>1035</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>556</v>
+        <v>1036</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>557</v>
+        <v>1037</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>558</v>
+        <v>1038</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>559</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="2">
@@ -2072,7 +3512,7 @@
         <v>2.5</v>
       </c>
       <c r="G2" s="0">
-        <v>-1.7126871789656586</v>
+        <v>-1.7126867935161019</v>
       </c>
       <c r="I2" s="0">
         <v>2.75</v>
@@ -2098,7 +3538,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="0">
-        <v>-0.63104865474908656</v>
+        <v>-0.63104806505054145</v>
       </c>
       <c r="I3" s="0">
         <v>19</v>
@@ -2124,7 +3564,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="0">
-        <v>-0.56580001268859614</v>
+        <v>-0.56580162699172865</v>
       </c>
       <c r="I4" s="0">
         <v>4.5</v>
@@ -2150,7 +3590,7 @@
         <v>3.5</v>
       </c>
       <c r="G5" s="0">
-        <v>1.1743166594743677</v>
+        <v>1.1743164139767108</v>
       </c>
       <c r="I5" s="0">
         <v>5</v>
@@ -2186,28 +3626,28 @@
   <sheetData>
     <row r="1">
       <c r="C1" s="0" t="s">
-        <v>560</v>
+        <v>1040</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>561</v>
+        <v>1041</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>562</v>
+        <v>1042</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>563</v>
+        <v>1043</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>564</v>
+        <v>1044</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>565</v>
+        <v>1045</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>566</v>
+        <v>1046</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>567</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="2">
@@ -2221,7 +3661,7 @@
         <v>1.25</v>
       </c>
       <c r="G2" s="0">
-        <v>-1.8540432888924869</v>
+        <v>-1.8540432777041265</v>
       </c>
       <c r="I2" s="0">
         <v>1.25</v>
@@ -2247,7 +3687,7 @@
         <v>2.5</v>
       </c>
       <c r="G3" s="0">
-        <v>-1.3286160509421336</v>
+        <v>-1.3286162054252855</v>
       </c>
       <c r="I3" s="0">
         <v>2.5</v>
@@ -2273,7 +3713,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="0">
-        <v>-1.7915219164974461</v>
+        <v>-1.7915218262850514</v>
       </c>
       <c r="I4" s="0">
         <v>4.25</v>
@@ -2299,7 +3739,7 @@
         <v>4.25</v>
       </c>
       <c r="G5" s="0">
-        <v>-1.7758214572301623</v>
+        <v>-1.7758205134671379</v>
       </c>
       <c r="I5" s="0">
         <v>9.75</v>
@@ -2335,28 +3775,28 @@
   <sheetData>
     <row r="1">
       <c r="C1" s="0" t="s">
-        <v>568</v>
+        <v>1048</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>569</v>
+        <v>1049</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>570</v>
+        <v>1050</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>571</v>
+        <v>1051</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>572</v>
+        <v>1052</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>573</v>
+        <v>1053</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>574</v>
+        <v>1054</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>575</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="2">
@@ -2370,7 +3810,7 @@
         <v>1.25</v>
       </c>
       <c r="G2" s="0">
-        <v>-2.0217378940567148</v>
+        <v>-2.0217378272971454</v>
       </c>
       <c r="I2" s="0">
         <v>1.25</v>
@@ -2396,7 +3836,7 @@
         <v>2.25</v>
       </c>
       <c r="G3" s="0">
-        <v>-1.0208207498234625</v>
+        <v>-1.0208214784690397</v>
       </c>
       <c r="I3" s="0">
         <v>2.5</v>
@@ -2422,7 +3862,7 @@
         <v>2.75</v>
       </c>
       <c r="G4" s="0">
-        <v>-1.4537957006556605</v>
+        <v>-1.453793144022097</v>
       </c>
       <c r="I4" s="0">
         <v>9.5</v>
@@ -2448,7 +3888,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="0">
-        <v>-0.8144167591121324</v>
+        <v>-0.81441358878887882</v>
       </c>
       <c r="I5" s="0">
         <v>4.25</v>
@@ -2484,28 +3924,28 @@
   <sheetData>
     <row r="1">
       <c r="C1" s="0" t="s">
-        <v>576</v>
+        <v>1056</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>577</v>
+        <v>1057</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>578</v>
+        <v>1058</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>579</v>
+        <v>1059</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>580</v>
+        <v>1060</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>581</v>
+        <v>1061</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>582</v>
+        <v>1062</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>583</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="2">
@@ -2519,7 +3959,7 @@
         <v>1.25</v>
       </c>
       <c r="G2" s="0">
-        <v>-1.7499656896565023</v>
+        <v>-1.7499657936861954</v>
       </c>
       <c r="I2" s="0">
         <v>1.25</v>
@@ -2545,7 +3985,7 @@
         <v>0.25</v>
       </c>
       <c r="G3" s="0">
-        <v>-0.56914806488746084</v>
+        <v>-0.56914844113724317</v>
       </c>
       <c r="I3" s="0">
         <v>2.5</v>
@@ -2571,7 +4011,7 @@
         <v>2.5</v>
       </c>
       <c r="G4" s="0">
-        <v>-1.4517713480960894</v>
+        <v>-1.4517710330254165</v>
       </c>
       <c r="I4" s="0">
         <v>4.25</v>
@@ -2597,7 +4037,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="0">
-        <v>-1.5651884273502523</v>
+        <v>-1.5651895822230766</v>
       </c>
       <c r="I5" s="0">
         <v>9.75</v>
@@ -2633,28 +4073,28 @@
   <sheetData>
     <row r="1">
       <c r="C1" s="0" t="s">
-        <v>584</v>
+        <v>1064</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>585</v>
+        <v>1065</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>586</v>
+        <v>1066</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>587</v>
+        <v>1067</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>588</v>
+        <v>1068</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>589</v>
+        <v>1069</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>590</v>
+        <v>1070</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>591</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="2">
@@ -2668,7 +4108,7 @@
         <v>1.25</v>
       </c>
       <c r="G2" s="0">
-        <v>-1.9110088038508335</v>
+        <v>-1.9110088146026338</v>
       </c>
       <c r="I2" s="0">
         <v>1.25</v>
@@ -2694,7 +4134,7 @@
         <v>2.5</v>
       </c>
       <c r="G3" s="0">
-        <v>-1.3422537671430457</v>
+        <v>-1.3422538837419919</v>
       </c>
       <c r="I3" s="0">
         <v>2.5</v>
@@ -2720,7 +4160,7 @@
         <v>4.25</v>
       </c>
       <c r="G4" s="0">
-        <v>-2.1904637395405357</v>
+        <v>-2.1904620195119979</v>
       </c>
       <c r="I4" s="0">
         <v>9.5</v>
@@ -2746,7 +4186,7 @@
         <v>5.5</v>
       </c>
       <c r="G5" s="0">
-        <v>-1.6229633559267818</v>
+        <v>-1.6229640685866491</v>
       </c>
       <c r="I5" s="0">
         <v>4.25</v>
@@ -2782,28 +4222,28 @@
   <sheetData>
     <row r="1">
       <c r="C1" s="0" t="s">
-        <v>592</v>
+        <v>1072</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>593</v>
+        <v>1073</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>594</v>
+        <v>1074</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>595</v>
+        <v>1075</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>596</v>
+        <v>1076</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>597</v>
+        <v>1077</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>598</v>
+        <v>1078</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>599</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="2">
@@ -2817,7 +4257,7 @@
         <v>1.25</v>
       </c>
       <c r="G2" s="0">
-        <v>-1.6732955613626572</v>
+        <v>-1.6732955387227721</v>
       </c>
       <c r="I2" s="0">
         <v>1.25</v>
@@ -2843,7 +4283,7 @@
         <v>2.5</v>
       </c>
       <c r="G3" s="0">
-        <v>-1.2218947325582961</v>
+        <v>-1.2218943892664469</v>
       </c>
       <c r="I3" s="0">
         <v>2.5</v>
@@ -2869,7 +4309,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="0">
-        <v>-1.5763578793003217</v>
+        <v>-1.5763581876640604</v>
       </c>
       <c r="I4" s="0">
         <v>4.25</v>
@@ -2895,7 +4335,7 @@
         <v>4.25</v>
       </c>
       <c r="G5" s="0">
-        <v>-0.86243110881354346</v>
+        <v>-0.86242997360532048</v>
       </c>
       <c r="I5" s="0">
         <v>9.75</v>
@@ -2931,28 +4371,28 @@
   <sheetData>
     <row r="1">
       <c r="C1" s="0" t="s">
-        <v>480</v>
+        <v>960</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>481</v>
+        <v>961</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>482</v>
+        <v>962</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>483</v>
+        <v>963</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>484</v>
+        <v>964</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>485</v>
+        <v>965</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>486</v>
+        <v>966</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>487</v>
+        <v>967</v>
       </c>
     </row>
     <row r="2">
@@ -2966,7 +4406,7 @@
         <v>1.25</v>
       </c>
       <c r="G2" s="0">
-        <v>-1.6220678664148063</v>
+        <v>-1.622067844836681</v>
       </c>
       <c r="I2" s="0">
         <v>1.25</v>
@@ -2992,7 +4432,7 @@
         <v>2.5</v>
       </c>
       <c r="G3" s="0">
-        <v>-1.2278818681266712</v>
+        <v>-1.227881485545729</v>
       </c>
       <c r="I3" s="0">
         <v>3</v>
@@ -3018,7 +4458,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="0">
-        <v>-1.2753748662573199</v>
+        <v>-1.2753753533414902</v>
       </c>
       <c r="I4" s="0">
         <v>4.25</v>
@@ -3044,7 +4484,7 @@
         <v>4.25</v>
       </c>
       <c r="G5" s="0">
-        <v>-0.22481759719823458</v>
+        <v>-0.22481640132984179</v>
       </c>
       <c r="I5" s="0">
         <v>10</v>
@@ -3080,28 +4520,28 @@
   <sheetData>
     <row r="1">
       <c r="C1" s="0" t="s">
-        <v>488</v>
+        <v>968</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>489</v>
+        <v>969</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>490</v>
+        <v>970</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>491</v>
+        <v>971</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>492</v>
+        <v>972</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>493</v>
+        <v>973</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>494</v>
+        <v>974</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>495</v>
+        <v>975</v>
       </c>
     </row>
     <row r="2">
@@ -3115,7 +4555,7 @@
         <v>1.25</v>
       </c>
       <c r="G2" s="0">
-        <v>-1.5407097228382098</v>
+        <v>-1.5407097056757548</v>
       </c>
       <c r="I2" s="0">
         <v>1.25</v>
@@ -3141,7 +4581,7 @@
         <v>2.5</v>
       </c>
       <c r="G3" s="0">
-        <v>-1.1867654581171569</v>
+        <v>-1.18676468408073</v>
       </c>
       <c r="I3" s="0">
         <v>2.75</v>
@@ -3167,7 +4607,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="0">
-        <v>-1.1019269706338977</v>
+        <v>-1.1019276306727022</v>
       </c>
       <c r="I4" s="0">
         <v>4</v>
@@ -3193,7 +4633,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="0">
-        <v>-2.3196207966709483</v>
+        <v>-2.3196215391398005</v>
       </c>
       <c r="I5" s="0">
         <v>10</v>
@@ -3229,28 +4669,28 @@
   <sheetData>
     <row r="1">
       <c r="C1" s="0" t="s">
-        <v>496</v>
+        <v>976</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>497</v>
+        <v>977</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>498</v>
+        <v>978</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>499</v>
+        <v>979</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>500</v>
+        <v>980</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>501</v>
+        <v>981</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>502</v>
+        <v>982</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>503</v>
+        <v>983</v>
       </c>
     </row>
     <row r="2">
@@ -3264,7 +4704,7 @@
         <v>1.25</v>
       </c>
       <c r="G2" s="0">
-        <v>-1.4708940731827902</v>
+        <v>-1.4708940539973323</v>
       </c>
       <c r="I2" s="0">
         <v>1.25</v>
@@ -3290,7 +4730,7 @@
         <v>0.75</v>
       </c>
       <c r="G3" s="0">
-        <v>-0.54343565217046463</v>
+        <v>-0.54343518371178456</v>
       </c>
       <c r="I3" s="0">
         <v>2.75</v>
@@ -3316,7 +4756,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="0">
-        <v>-2.0489608426792958</v>
+        <v>-2.0489613992828142</v>
       </c>
       <c r="I4" s="0">
         <v>4</v>
@@ -3342,7 +4782,7 @@
         <v>3.25</v>
       </c>
       <c r="G5" s="0">
-        <v>-1.3636936418704377</v>
+        <v>-1.3636940624432199</v>
       </c>
       <c r="I5" s="0">
         <v>4.5</v>
@@ -3378,28 +4818,28 @@
   <sheetData>
     <row r="1">
       <c r="C1" s="0" t="s">
-        <v>504</v>
+        <v>984</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>505</v>
+        <v>985</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>506</v>
+        <v>986</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>507</v>
+        <v>987</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>508</v>
+        <v>988</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>509</v>
+        <v>989</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>510</v>
+        <v>990</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>511</v>
+        <v>991</v>
       </c>
     </row>
     <row r="2">
@@ -3413,7 +4853,7 @@
         <v>1.25</v>
       </c>
       <c r="G2" s="0">
-        <v>-1.7289842130423403</v>
+        <v>-1.728984080136392</v>
       </c>
       <c r="I2" s="0">
         <v>1.25</v>
@@ -3439,7 +4879,7 @@
         <v>2.5</v>
       </c>
       <c r="G3" s="0">
-        <v>-1.6523142501566335</v>
+        <v>-1.6523143619035197</v>
       </c>
       <c r="I3" s="0">
         <v>2.5</v>
@@ -3465,7 +4905,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="0">
-        <v>-1.8847539066961609</v>
+        <v>-1.8847538589701307</v>
       </c>
       <c r="I4" s="0">
         <v>4.25</v>
@@ -3491,7 +4931,7 @@
         <v>4.25</v>
       </c>
       <c r="G5" s="0">
-        <v>-0.79775780026360077</v>
+        <v>-0.79775686484013897</v>
       </c>
       <c r="I5" s="0">
         <v>10</v>
@@ -3527,28 +4967,28 @@
   <sheetData>
     <row r="1">
       <c r="C1" s="0" t="s">
-        <v>512</v>
+        <v>992</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>513</v>
+        <v>993</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>514</v>
+        <v>994</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>515</v>
+        <v>995</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>516</v>
+        <v>996</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>517</v>
+        <v>997</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>518</v>
+        <v>998</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>519</v>
+        <v>999</v>
       </c>
     </row>
     <row r="2">
@@ -3562,7 +5002,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="0">
-        <v>-1.5585475493123571</v>
+        <v>-1.5585639129030906</v>
       </c>
       <c r="I2" s="0">
         <v>2.75</v>
@@ -3588,7 +5028,7 @@
         <v>3.75</v>
       </c>
       <c r="G3" s="0">
-        <v>-0.96294516832279653</v>
+        <v>-0.96297455528880782</v>
       </c>
       <c r="I3" s="0">
         <v>6</v>
@@ -3614,7 +5054,7 @@
         <v>9</v>
       </c>
       <c r="G4" s="0">
-        <v>-1.8298913084013058</v>
+        <v>-1.8298292632723394</v>
       </c>
       <c r="I4" s="0">
         <v>15.25</v>
@@ -3640,7 +5080,7 @@
         <v>12</v>
       </c>
       <c r="G5" s="0">
-        <v>-1.4589007962907632</v>
+        <v>-1.4587766137729079</v>
       </c>
       <c r="I5" s="0">
         <v>8.75</v>
@@ -3676,28 +5116,28 @@
   <sheetData>
     <row r="1">
       <c r="C1" s="0" t="s">
-        <v>520</v>
+        <v>1000</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>521</v>
+        <v>1001</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>522</v>
+        <v>1002</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>523</v>
+        <v>1003</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>524</v>
+        <v>1004</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>525</v>
+        <v>1005</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>526</v>
+        <v>1006</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>527</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="2">
@@ -3711,7 +5151,7 @@
         <v>9.75</v>
       </c>
       <c r="G2" s="0">
-        <v>-1.2033619153964221</v>
+        <v>-1.2033950144945575</v>
       </c>
       <c r="I2" s="0">
         <v>2.75</v>
@@ -3737,7 +5177,7 @@
         <v>31.5</v>
       </c>
       <c r="G3" s="0">
-        <v>-1.5483116579599387</v>
+        <v>-1.5483161399697358</v>
       </c>
       <c r="I3" s="0">
         <v>4.75</v>
@@ -3763,7 +5203,7 @@
         <v>33</v>
       </c>
       <c r="G4" s="0">
-        <v>-1.5491031198088698</v>
+        <v>-1.549109251454005</v>
       </c>
       <c r="I4" s="0">
         <v>6.25</v>
@@ -3789,7 +5229,7 @@
         <v>33.75</v>
       </c>
       <c r="G5" s="0">
-        <v>-1.5502342049499223</v>
+        <v>-1.5502394133108464</v>
       </c>
       <c r="I5" s="0">
         <v>9.5</v>
@@ -3825,28 +5265,28 @@
   <sheetData>
     <row r="1">
       <c r="C1" s="0" t="s">
-        <v>528</v>
+        <v>1008</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>529</v>
+        <v>1009</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>530</v>
+        <v>1010</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>531</v>
+        <v>1011</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>532</v>
+        <v>1012</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>533</v>
+        <v>1013</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>534</v>
+        <v>1014</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>535</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="2">
@@ -3860,7 +5300,7 @@
         <v>9.75</v>
       </c>
       <c r="G2" s="0">
-        <v>-1.2338716352784389</v>
+        <v>-1.233915140799374</v>
       </c>
       <c r="I2" s="0">
         <v>2.5</v>
@@ -3886,7 +5326,7 @@
         <v>42.75</v>
       </c>
       <c r="G3" s="0">
-        <v>-1.5575907144416019</v>
+        <v>-1.5575904508005807</v>
       </c>
       <c r="I3" s="0">
         <v>4.75</v>
@@ -3912,7 +5352,7 @@
         <v>49.25</v>
       </c>
       <c r="G4" s="0">
-        <v>-1.5504827016028391</v>
+        <v>-1.5504830989631835</v>
       </c>
       <c r="I4" s="0">
         <v>6.25</v>
@@ -3938,7 +5378,7 @@
         <v>53</v>
       </c>
       <c r="G5" s="0">
-        <v>-1.5503360096097409</v>
+        <v>-1.5503361131715094</v>
       </c>
       <c r="I5" s="0">
         <v>9.5</v>
@@ -3974,28 +5414,28 @@
   <sheetData>
     <row r="1">
       <c r="C1" s="0" t="s">
-        <v>536</v>
+        <v>1016</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>537</v>
+        <v>1017</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>538</v>
+        <v>1018</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>539</v>
+        <v>1019</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>540</v>
+        <v>1020</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>541</v>
+        <v>1021</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>542</v>
+        <v>1022</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>543</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="2">
@@ -4009,7 +5449,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="0">
-        <v>-1.131175216992901</v>
+        <v>-1.1311639423498705</v>
       </c>
       <c r="I2" s="0">
         <v>2.5</v>
@@ -4035,7 +5475,7 @@
         <v>5.75</v>
       </c>
       <c r="G3" s="0">
-        <v>-0.6407426839321505</v>
+        <v>-0.64075721734969093</v>
       </c>
       <c r="I3" s="0">
         <v>0.75</v>
@@ -4061,7 +5501,7 @@
         <v>10.5</v>
       </c>
       <c r="G4" s="0">
-        <v>-1.4851321865143476</v>
+        <v>-1.4850947863609913</v>
       </c>
       <c r="I4" s="0">
         <v>4</v>
@@ -4087,7 +5527,7 @@
         <v>12</v>
       </c>
       <c r="G5" s="0">
-        <v>-1.4695528241220253</v>
+        <v>-1.4696579450421168</v>
       </c>
       <c r="I5" s="0">
         <v>5.75</v>

</xml_diff>